<commit_message>
changes in visualization and auto_trainer
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -480,16 +480,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.73</v>
+        <v>0.7533</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7047</v>
+        <v>0.7151999999999999</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7393999999999999</v>
+        <v>0.7958</v>
       </c>
       <c r="G2" t="n">
-        <v>0.7216</v>
+        <v>0.7533</v>
       </c>
     </row>
   </sheetData>

</xml_diff>